<commit_message>
Fix ANV code and regenerate objects, fix mainrun automl code
</commit_message>
<xml_diff>
--- a/26_PredictingCp/gcd_ml_features.xlsx
+++ b/26_PredictingCp/gcd_ml_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ltamon/SahakyanLab/GenomicContactDynamics/26_PredictingCp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918A9E10-76EA-2C4E-A53D-CB826AE70EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0804DD2B-0A8D-4247-9EA0-B5050E8CCFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="960" windowWidth="33600" windowHeight="19200" xr2:uid="{AA5E7137-4ED1-AA41-84AB-4DC9971FDF4E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Feature</t>
   </si>
@@ -107,6 +107,27 @@
   </si>
   <si>
     <t>exclude</t>
+  </si>
+  <si>
+    <t>grp.compl.</t>
+  </si>
+  <si>
+    <t>grp.kmer3.</t>
+  </si>
+  <si>
+    <t>grp.kmer1.</t>
+  </si>
+  <si>
+    <t>grp.GC.ij</t>
+  </si>
+  <si>
+    <t>grp.GC.j_</t>
+  </si>
+  <si>
+    <t>grp.GC.i_</t>
+  </si>
+  <si>
+    <t>grp.anv.</t>
   </si>
 </sst>
 </file>
@@ -465,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633D6BD0-1E6A-CB46-BF76-A7DB025BF8B9}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,7 +498,7 @@
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -510,8 +531,11 @@
       <c r="F2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -530,8 +554,11 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -550,8 +577,11 @@
       <c r="F4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -570,8 +600,11 @@
       <c r="F5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -590,8 +623,11 @@
       <c r="F6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -611,8 +647,11 @@
       <c r="F7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -625,8 +664,11 @@
       <c r="F8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -646,8 +688,14 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -668,10 +716,13 @@
         <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -679,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>

</xml_diff>